<commit_message>
Upload completed reproducibility checklist
</commit_message>
<xml_diff>
--- a/osfstorage-archive/Papers for the exercise/Paper 2/Reproducibility checklist - Paper 2.xlsx
+++ b/osfstorage-archive/Papers for the exercise/Paper 2/Reproducibility checklist - Paper 2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucijabatinovic/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ndporter/Desktop/Papers for the exercise/Paper 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FAED42E-95C4-1F45-B984-C05004384F12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A21BCBD7-9AD5-B24C-97E7-C802200AFEEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="500" windowWidth="27800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="74120" yWindow="13720" windowWidth="39960" windowHeight="23820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Protocol" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="62">
   <si>
     <t>Reproducibility check</t>
   </si>
@@ -51,9 +51,6 @@
   </si>
   <si>
     <t>Can the data be read using software indicated by author?</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
   <si>
     <t>Are the data in archive-ready formats (CSV, TXT)?</t>
@@ -173,16 +170,62 @@
   <si>
     <t>Cite this page as: Social Science Data Editors. 2021. "Verification guidance". Data and Code Guidance by Data Editors. Accessed at https://social-science-data-editors.github.io/guidance/Verification_guidance.html on 2021-04-30.</t>
   </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Handedness is classified differently in code from reported values in table 1 and table 2.</t>
+  </si>
+  <si>
+    <t>Figure proportions are different for all figures but reproduces otherwise correctly</t>
+  </si>
+  <si>
+    <t>Rstudio, R 4.2.2, Windows (Ana can add more detail if needed)</t>
+  </si>
+  <si>
+    <t>Differences in mean age (Table 1) for Studies 1 and 3</t>
+  </si>
+  <si>
+    <t>Total N=2,314 not in knit output (but can be verified by manually reading the data); can't find direct code for study 1 showing "extremely left-handed females" (n=3) other than scatterplot that is not by gender</t>
+  </si>
+  <si>
+    <t>Any results that are not in the paper ideally shouldn't be in the reproduction code</t>
+  </si>
+  <si>
+    <t>Additional Comments:</t>
+  </si>
+  <si>
+    <t>Ana Martinovici, Nathaniel Porter</t>
+  </si>
+  <si>
+    <t>Ideally the code should use the version of data stored in the package (currently reads from a github repo) although the files are identical</t>
+  </si>
+  <si>
+    <t>Martinovici@rsm.nl; ndporter@vt.edu</t>
+  </si>
+  <si>
+    <t>Reproduction attempt at https://github.com/anamartinovici/OS_conf-reproducibility</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -235,9 +278,12 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
-      <name val="Calibri"/>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -290,43 +336,55 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -366,7 +424,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp14.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp15.xml><?xml version="1.0" encoding="utf-8"?>
@@ -378,7 +436,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -390,11 +448,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
@@ -434,7 +492,7 @@
                   <a14:compatExt spid="_x0000_s1028"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E00A3575-40DC-C9A4-BA6C-80112AD3677C}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -480,14 +538,19 @@
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>254000</xdr:colOff>
           <xdr:row>31</xdr:row>
           <xdr:rowOff>76200</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="330200" cy="381000"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>584200</xdr:colOff>
+          <xdr:row>33</xdr:row>
+          <xdr:rowOff>101600</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1029" name="Check Box 5" hidden="1">
@@ -496,7 +559,7 @@
                   <a14:compatExt spid="_x0000_s1029"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9BCC4E87-58E7-1E4B-8819-18F41BBEAE78}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -536,20 +599,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>254000</xdr:colOff>
           <xdr:row>32</xdr:row>
           <xdr:rowOff>76200</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="330200" cy="381000"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>584200</xdr:colOff>
+          <xdr:row>34</xdr:row>
+          <xdr:rowOff>101600</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1030" name="Check Box 6" hidden="1">
@@ -558,7 +626,7 @@
                   <a14:compatExt spid="_x0000_s1030"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D2BE0FCA-8291-964F-9886-42AC37156E61}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -598,20 +666,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>254000</xdr:colOff>
           <xdr:row>33</xdr:row>
           <xdr:rowOff>76200</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="330200" cy="381000"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>584200</xdr:colOff>
+          <xdr:row>35</xdr:row>
+          <xdr:rowOff>101600</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1031" name="Check Box 7" hidden="1">
@@ -620,7 +693,7 @@
                   <a14:compatExt spid="_x0000_s1031"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2EE72A3F-F199-6E48-B4B9-DCBCAC4BC3ED}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -660,20 +733,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>254000</xdr:colOff>
           <xdr:row>35</xdr:row>
           <xdr:rowOff>76200</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="330200" cy="381000"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>584200</xdr:colOff>
+          <xdr:row>37</xdr:row>
+          <xdr:rowOff>101600</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1032" name="Check Box 8" hidden="1">
@@ -682,7 +760,7 @@
                   <a14:compatExt spid="_x0000_s1032"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2525B164-C614-584F-87CD-5BBD79F60DAC}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -722,20 +800,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>254000</xdr:colOff>
           <xdr:row>36</xdr:row>
           <xdr:rowOff>76200</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="330200" cy="381000"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>584200</xdr:colOff>
+          <xdr:row>38</xdr:row>
+          <xdr:rowOff>101600</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1033" name="Check Box 9" hidden="1">
@@ -744,7 +827,7 @@
                   <a14:compatExt spid="_x0000_s1033"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60363739-56EE-1A48-B163-4DC179139CA3}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -784,20 +867,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>254000</xdr:colOff>
           <xdr:row>37</xdr:row>
           <xdr:rowOff>76200</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="330200" cy="381000"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>584200</xdr:colOff>
+          <xdr:row>39</xdr:row>
+          <xdr:rowOff>101600</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1034" name="Check Box 10" hidden="1">
@@ -806,7 +894,7 @@
                   <a14:compatExt spid="_x0000_s1034"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40C63110-2538-4147-B954-5618379DC106}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -846,20 +934,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>254000</xdr:colOff>
           <xdr:row>38</xdr:row>
           <xdr:rowOff>76200</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="330200" cy="381000"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>584200</xdr:colOff>
+          <xdr:row>40</xdr:row>
+          <xdr:rowOff>101600</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1035" name="Check Box 11" hidden="1">
@@ -868,7 +961,7 @@
                   <a14:compatExt spid="_x0000_s1035"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3064CD80-BB3C-A04B-87AD-BB8668448C12}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -908,20 +1001,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>254000</xdr:colOff>
           <xdr:row>39</xdr:row>
           <xdr:rowOff>76200</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="330200" cy="381000"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>584200</xdr:colOff>
+          <xdr:row>41</xdr:row>
+          <xdr:rowOff>101600</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1036" name="Check Box 12" hidden="1">
@@ -930,7 +1028,7 @@
                   <a14:compatExt spid="_x0000_s1036"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B51C871-1302-EB45-8C32-E2228531D667}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -970,20 +1068,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>254000</xdr:colOff>
           <xdr:row>40</xdr:row>
           <xdr:rowOff>76200</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="330200" cy="381000"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>584200</xdr:colOff>
+          <xdr:row>41</xdr:row>
+          <xdr:rowOff>279400</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1037" name="Check Box 13" hidden="1">
@@ -992,7 +1095,7 @@
                   <a14:compatExt spid="_x0000_s1037"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0BC84B9-934B-6A48-A7DF-53006B3623FF}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1032,20 +1135,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>254000</xdr:colOff>
           <xdr:row>42</xdr:row>
           <xdr:rowOff>76200</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="330200" cy="381000"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>584200</xdr:colOff>
+          <xdr:row>42</xdr:row>
+          <xdr:rowOff>457200</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1039" name="Check Box 15" hidden="1">
@@ -1054,7 +1162,7 @@
                   <a14:compatExt spid="_x0000_s1039"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F84D3AA-0EC3-EB46-9B3A-1ADB946F5E5C}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1094,20 +1202,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>254000</xdr:colOff>
           <xdr:row>43</xdr:row>
           <xdr:rowOff>76200</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="330200" cy="381000"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>584200</xdr:colOff>
+          <xdr:row>44</xdr:row>
+          <xdr:rowOff>101600</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1040" name="Check Box 16" hidden="1">
@@ -1116,7 +1229,7 @@
                   <a14:compatExt spid="_x0000_s1040"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2586CA96-BA15-C642-9289-40F6F52AD702}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000010040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1156,20 +1269,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>254000</xdr:colOff>
           <xdr:row>16</xdr:row>
           <xdr:rowOff>76200</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="330200" cy="381000"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>584200</xdr:colOff>
+          <xdr:row>18</xdr:row>
+          <xdr:rowOff>114300</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1041" name="Check Box 17" hidden="1">
@@ -1178,7 +1296,7 @@
                   <a14:compatExt spid="_x0000_s1041"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FDF4E8B0-A71A-3F47-A7A4-50ED52AE830A}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000011040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1218,20 +1336,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>254000</xdr:colOff>
           <xdr:row>17</xdr:row>
           <xdr:rowOff>76200</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="330200" cy="381000"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>584200</xdr:colOff>
+          <xdr:row>19</xdr:row>
+          <xdr:rowOff>101600</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1042" name="Check Box 18" hidden="1">
@@ -1240,7 +1363,7 @@
                   <a14:compatExt spid="_x0000_s1042"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C625516A-D1A5-C543-BAD5-E23DA352CD1D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000012040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1280,20 +1403,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>254000</xdr:colOff>
           <xdr:row>18</xdr:row>
           <xdr:rowOff>76200</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="330200" cy="381000"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>584200</xdr:colOff>
+          <xdr:row>20</xdr:row>
+          <xdr:rowOff>101600</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1043" name="Check Box 19" hidden="1">
@@ -1302,7 +1430,7 @@
                   <a14:compatExt spid="_x0000_s1043"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94BA7CDE-9EA3-0449-854F-697AD7E9CF1A}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000013040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1342,20 +1470,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>254000</xdr:colOff>
           <xdr:row>19</xdr:row>
           <xdr:rowOff>76200</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="330200" cy="381000"/>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>584200</xdr:colOff>
+          <xdr:row>21</xdr:row>
+          <xdr:rowOff>101600</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1044" name="Check Box 20" hidden="1">
@@ -1364,7 +1497,7 @@
                   <a14:compatExt spid="_x0000_s1044"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C675BF5-3620-7C46-968A-3F433A21B7D2}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000014040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1404,7 +1537,7 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
@@ -1614,9 +1747,9 @@
   </sheetPr>
   <dimension ref="A1:C1005"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1627,7 +1760,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="27.75" customHeight="1">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="11"/>
@@ -1643,28 +1776,32 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="14">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="10" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
     </row>
-    <row r="4" spans="1:3" ht="16">
+    <row r="4" spans="1:3" ht="17">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-    </row>
-    <row r="5" spans="1:3" ht="16">
+      <c r="C4" s="16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="17">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
+      <c r="C5" s="16" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="6" spans="1:3" ht="14">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="11"/>
@@ -1678,7 +1815,7 @@
       <c r="C7" s="4"/>
     </row>
     <row r="8" spans="1:3" ht="14">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="10" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="11"/>
@@ -1689,274 +1826,283 @@
         <v>9</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="5"/>
+    </row>
+    <row r="10" spans="1:3" ht="14">
+      <c r="A10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="5"/>
-    </row>
-    <row r="10" spans="1:3" ht="14">
-      <c r="A10" s="5" t="s">
-        <v>11</v>
-      </c>
       <c r="B10" s="5" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="C10" s="5"/>
     </row>
     <row r="11" spans="1:3" ht="14">
-      <c r="A11" s="12" t="s">
-        <v>12</v>
+      <c r="A11" s="10" t="s">
+        <v>11</v>
       </c>
       <c r="B11" s="11"/>
       <c r="C11" s="11"/>
     </row>
     <row r="12" spans="1:3" ht="13">
       <c r="A12" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
     </row>
-    <row r="13" spans="1:3" ht="14">
+    <row r="13" spans="1:3" ht="28">
       <c r="A13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="28">
+      <c r="A14" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>10</v>
+      <c r="B14" s="5" t="s">
+        <v>50</v>
       </c>
-      <c r="C13" s="6"/>
-    </row>
-    <row r="14" spans="1:3" ht="14">
-      <c r="A14" s="6" t="s">
+      <c r="C14" s="15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="70">
+      <c r="A15" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>10</v>
+      <c r="B15" s="5" t="s">
+        <v>50</v>
       </c>
-      <c r="C14" s="6"/>
-    </row>
-    <row r="15" spans="1:3" ht="14">
-      <c r="A15" s="6" t="s">
+      <c r="C15" s="15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="14">
+      <c r="A16" s="10" t="s">
         <v>16</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="6"/>
-    </row>
-    <row r="16" spans="1:3" ht="14">
-      <c r="A16" s="12" t="s">
-        <v>17</v>
       </c>
       <c r="B16" s="11"/>
       <c r="C16" s="11"/>
     </row>
     <row r="17" spans="1:3" ht="13">
-      <c r="A17" s="10" t="s">
-        <v>18</v>
+      <c r="A17" s="14" t="s">
+        <v>17</v>
       </c>
       <c r="B17" s="11"/>
       <c r="C17" s="11"/>
     </row>
     <row r="18" spans="1:3" ht="14">
       <c r="A18" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
     </row>
     <row r="19" spans="1:3" ht="14">
       <c r="A19" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
     </row>
     <row r="20" spans="1:3" ht="14">
       <c r="A20" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
     </row>
     <row r="21" spans="1:3" ht="14">
       <c r="A21" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
     </row>
     <row r="22" spans="1:3" ht="14">
-      <c r="A22" s="12" t="s">
-        <v>23</v>
+      <c r="A22" s="10" t="s">
+        <v>22</v>
       </c>
       <c r="B22" s="11"/>
       <c r="C22" s="11"/>
     </row>
     <row r="23" spans="1:3" ht="14">
       <c r="A23" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="C23" s="5"/>
     </row>
     <row r="24" spans="1:3" ht="14">
-      <c r="A24" s="12" t="s">
-        <v>25</v>
+      <c r="A24" s="10" t="s">
+        <v>24</v>
       </c>
       <c r="B24" s="11"/>
       <c r="C24" s="11"/>
     </row>
     <row r="25" spans="1:3" ht="28">
       <c r="A25" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
+      <c r="C25" s="17" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="26" spans="1:3" ht="14">
-      <c r="A26" s="12" t="s">
-        <v>27</v>
+      <c r="A26" s="10" t="s">
+        <v>26</v>
       </c>
       <c r="B26" s="11"/>
       <c r="C26" s="11"/>
     </row>
     <row r="27" spans="1:3" ht="13">
       <c r="A27" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B27" s="11"/>
       <c r="C27" s="11"/>
     </row>
     <row r="28" spans="1:3" ht="14">
       <c r="A28" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="28">
+      <c r="A29" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="5" t="s">
-        <v>10</v>
+      <c r="B29" s="5" t="s">
+        <v>50</v>
       </c>
-      <c r="C28" s="5"/>
-    </row>
-    <row r="29" spans="1:3" ht="28">
-      <c r="A29" s="5" t="s">
+      <c r="C29" s="17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="14">
+      <c r="A30" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B29" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C29" s="5"/>
-    </row>
-    <row r="30" spans="1:3" ht="14">
-      <c r="A30" s="6" t="s">
-        <v>31</v>
-      </c>
       <c r="B30" s="5" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="C30" s="5"/>
     </row>
     <row r="31" spans="1:3" ht="14">
-      <c r="A31" s="12" t="s">
-        <v>32</v>
+      <c r="A31" s="10" t="s">
+        <v>31</v>
       </c>
       <c r="B31" s="11"/>
       <c r="C31" s="11"/>
     </row>
     <row r="32" spans="1:3" ht="14">
       <c r="A32" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
     </row>
     <row r="33" spans="1:3" ht="14">
       <c r="A33" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
     </row>
     <row r="34" spans="1:3" ht="14">
       <c r="A34" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
     </row>
     <row r="35" spans="1:3" ht="14">
       <c r="A35" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
     </row>
     <row r="36" spans="1:3" ht="14">
-      <c r="A36" s="12" t="s">
-        <v>37</v>
+      <c r="A36" s="10" t="s">
+        <v>36</v>
       </c>
       <c r="B36" s="11"/>
       <c r="C36" s="11"/>
     </row>
     <row r="37" spans="1:3" ht="14">
       <c r="A37" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
     </row>
     <row r="38" spans="1:3" ht="14">
       <c r="A38" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
     </row>
     <row r="39" spans="1:3" ht="14">
       <c r="A39" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
     </row>
     <row r="40" spans="1:3" ht="14">
       <c r="A40" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
     </row>
     <row r="41" spans="1:3" ht="14">
       <c r="A41" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
     </row>
     <row r="42" spans="1:3" ht="42">
       <c r="A42" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
     </row>
     <row r="43" spans="1:3" ht="56">
       <c r="A43" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
     </row>
     <row r="44" spans="1:3" ht="28">
       <c r="A44" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
     </row>
     <row r="45" spans="1:3" ht="14">
       <c r="A45" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
@@ -1971,23 +2117,31 @@
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
     </row>
-    <row r="48" spans="1:3" ht="13">
-      <c r="A48" s="5"/>
+    <row r="48" spans="1:3" ht="14">
+      <c r="A48" s="18" t="s">
+        <v>57</v>
+      </c>
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
     </row>
-    <row r="49" spans="1:3" ht="13">
-      <c r="A49" s="5"/>
+    <row r="49" spans="1:3" ht="14">
+      <c r="A49" s="18" t="s">
+        <v>56</v>
+      </c>
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
     </row>
-    <row r="50" spans="1:3" ht="13">
-      <c r="A50" s="5"/>
+    <row r="50" spans="1:3" ht="28">
+      <c r="A50" s="18" t="s">
+        <v>59</v>
+      </c>
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
     </row>
-    <row r="51" spans="1:3" ht="13">
-      <c r="A51" s="5"/>
+    <row r="51" spans="1:3" ht="14">
+      <c r="A51" s="18" t="s">
+        <v>61</v>
+      </c>
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
     </row>
@@ -7163,15 +7317,15 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1">
       <c r="A1" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A2" s="8" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A2" s="8" t="s">
+      <c r="B2" s="9" t="s">
         <v>48</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>